<commit_message>
Updated to end of 2016 season
</commit_message>
<xml_diff>
--- a/Tournament Results.xlsx
+++ b/Tournament Results.xlsx
@@ -42507,6 +42507,1011 @@
         <v>122</v>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>122.472408880856</v>
+      </c>
+      <c r="C125" t="n">
+        <v>94.6831103934111</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0.731504316498081</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.603121914343077</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0.790876256090942</v>
+      </c>
+      <c r="G125" t="n">
+        <v>110.797185112423</v>
+      </c>
+      <c r="H125" t="n">
+        <v>99.2863885840249</v>
+      </c>
+      <c r="I125" t="n">
+        <v>71.7572758629269</v>
+      </c>
+      <c r="J125" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="K125" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="L125" t="n">
+        <v>61.1</v>
+      </c>
+      <c r="M125" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="N125" t="n">
+        <v>19</v>
+      </c>
+      <c r="O125" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="P125" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>54.1</v>
+      </c>
+      <c r="R125" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="S125" t="n">
+        <v>112.1</v>
+      </c>
+      <c r="T125" t="n">
+        <v>64</v>
+      </c>
+      <c r="U125" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="V125" t="n">
+        <v>39.7</v>
+      </c>
+      <c r="W125" t="n">
+        <v>73.4</v>
+      </c>
+      <c r="X125" t="n">
+        <v>55.7</v>
+      </c>
+      <c r="Y125" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="Z125" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="AA125" t="n">
+        <v>1.656</v>
+      </c>
+      <c r="AB125" t="n">
+        <v>0.575</v>
+      </c>
+      <c r="AC125" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="AD125" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="AE125" t="n">
+        <v>-13.1</v>
+      </c>
+      <c r="AF125" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="AG125" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="AH125" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI125" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="AJ125" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="AK125" t="n">
+        <v>36</v>
+      </c>
+      <c r="AL125" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="AM125" t="n">
+        <v>70.2</v>
+      </c>
+      <c r="AN125" t="n">
+        <v>102.2</v>
+      </c>
+      <c r="AO125" t="n">
+        <v>59.7</v>
+      </c>
+      <c r="AP125" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="AQ125" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="AR125" t="n">
+        <v>60.3</v>
+      </c>
+      <c r="AS125" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="AT125" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AU125" t="n">
+        <v>0.863</v>
+      </c>
+      <c r="AV125" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="AW125" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="AX125" t="n">
+        <v>21.8</v>
+      </c>
+      <c r="AY125" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="AZ125" t="n">
+        <v>1.027</v>
+      </c>
+      <c r="BA125" t="n">
+        <v>0.949</v>
+      </c>
+      <c r="BB125" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="BC125" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="BD125" t="s">
+        <v>203</v>
+      </c>
+      <c r="BE125" t="n">
+        <v>111.887498470978</v>
+      </c>
+      <c r="BF125" t="n">
+        <v>93.2967229009327</v>
+      </c>
+      <c r="BG125" t="n">
+        <v>0.700702559833434</v>
+      </c>
+      <c r="BH125" t="n">
+        <v>0.517936613792802</v>
+      </c>
+      <c r="BI125" t="n">
+        <v>0.794525575768337</v>
+      </c>
+      <c r="BJ125" t="n">
+        <v>110.052235729994</v>
+      </c>
+      <c r="BK125" t="n">
+        <v>99.452497067608</v>
+      </c>
+      <c r="BL125" t="n">
+        <v>65.4975872773356</v>
+      </c>
+      <c r="BM125" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="BN125" t="n">
+        <v>48.3</v>
+      </c>
+      <c r="BO125" t="n">
+        <v>43.6</v>
+      </c>
+      <c r="BP125" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="BQ125" t="n">
+        <v>19.9</v>
+      </c>
+      <c r="BR125" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="BS125" t="n">
+        <v>36.1</v>
+      </c>
+      <c r="BT125" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="BU125" t="n">
+        <v>69.4</v>
+      </c>
+      <c r="BV125" t="n">
+        <v>107</v>
+      </c>
+      <c r="BW125" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="BX125" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="BY125" t="n">
+        <v>31.7</v>
+      </c>
+      <c r="BZ125" t="n">
+        <v>67</v>
+      </c>
+      <c r="CA125" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="CB125" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="CC125" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="CD125" t="n">
+        <v>1.143</v>
+      </c>
+      <c r="CE125" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="CF125" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="CG125" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="CH125" t="n">
+        <v>-5.5</v>
+      </c>
+      <c r="CI125" t="n">
+        <v>44.9</v>
+      </c>
+      <c r="CJ125" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="CK125" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="CL125" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="CM125" t="n">
+        <v>47</v>
+      </c>
+      <c r="CN125" t="n">
+        <v>30.8</v>
+      </c>
+      <c r="CO125" t="n">
+        <v>47.6</v>
+      </c>
+      <c r="CP125" t="n">
+        <v>66.3</v>
+      </c>
+      <c r="CQ125" t="n">
+        <v>99.4</v>
+      </c>
+      <c r="CR125" t="n">
+        <v>57.3</v>
+      </c>
+      <c r="CS125" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="CT125" t="n">
+        <v>33</v>
+      </c>
+      <c r="CU125" t="n">
+        <v>68.3</v>
+      </c>
+      <c r="CV125" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="CW125" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="CX125" t="n">
+        <v>1.152</v>
+      </c>
+      <c r="CY125" t="n">
+        <v>0.656</v>
+      </c>
+      <c r="CZ125" t="n">
+        <v>17</v>
+      </c>
+      <c r="DA125" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="DB125" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="DC125" t="n">
+        <v>0.976</v>
+      </c>
+      <c r="DD125" t="n">
+        <v>0.964</v>
+      </c>
+      <c r="DE125" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="DF125" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="DG125" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>159</v>
+      </c>
+      <c r="B126" t="n">
+        <v>118.70227059828</v>
+      </c>
+      <c r="C126" t="n">
+        <v>93.1606214962715</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.75453708018108</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0.563394891283762</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0.839881470981451</v>
+      </c>
+      <c r="G126" t="n">
+        <v>110.708500425401</v>
+      </c>
+      <c r="H126" t="n">
+        <v>97.7125081879537</v>
+      </c>
+      <c r="I126" t="n">
+        <v>70.901528263298</v>
+      </c>
+      <c r="J126" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="K126" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="L126" t="n">
+        <v>43</v>
+      </c>
+      <c r="M126" t="n">
+        <v>38.9</v>
+      </c>
+      <c r="N126" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="O126" t="n">
+        <v>54.8</v>
+      </c>
+      <c r="P126" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>48.4</v>
+      </c>
+      <c r="R126" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="S126" t="n">
+        <v>115.5</v>
+      </c>
+      <c r="T126" t="n">
+        <v>60.1</v>
+      </c>
+      <c r="U126" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="V126" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="W126" t="n">
+        <v>72</v>
+      </c>
+      <c r="X126" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="Y126" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="Z126" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA126" t="n">
+        <v>1.138</v>
+      </c>
+      <c r="AB126" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="AC126" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="AD126" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="AE126" t="n">
+        <v>-10.1</v>
+      </c>
+      <c r="AF126" t="n">
+        <v>44.9</v>
+      </c>
+      <c r="AG126" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="AH126" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="AI126" t="n">
+        <v>17</v>
+      </c>
+      <c r="AJ126" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="AK126" t="n">
+        <v>33.1</v>
+      </c>
+      <c r="AL126" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="AM126" t="n">
+        <v>67.7</v>
+      </c>
+      <c r="AN126" t="n">
+        <v>98.7</v>
+      </c>
+      <c r="AO126" t="n">
+        <v>62.9</v>
+      </c>
+      <c r="AP126" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="AQ126" t="n">
+        <v>28</v>
+      </c>
+      <c r="AR126" t="n">
+        <v>70.4</v>
+      </c>
+      <c r="AS126" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="AT126" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="AU126" t="n">
+        <v>0.869</v>
+      </c>
+      <c r="AV126" t="n">
+        <v>0.432</v>
+      </c>
+      <c r="AW126" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="AX126" t="n">
+        <v>22.9</v>
+      </c>
+      <c r="AY126" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="AZ126" t="n">
+        <v>0.953</v>
+      </c>
+      <c r="BA126" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="BB126" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="BC126" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="BD126" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE126" t="n">
+        <v>121.607651393701</v>
+      </c>
+      <c r="BF126" t="n">
+        <v>90.9489303078528</v>
+      </c>
+      <c r="BG126" t="n">
+        <v>0.711354159630472</v>
+      </c>
+      <c r="BH126" t="n">
+        <v>0.588242734646016</v>
+      </c>
+      <c r="BI126" t="n">
+        <v>0.752598454548143</v>
+      </c>
+      <c r="BJ126" t="n">
+        <v>109.45666079805</v>
+      </c>
+      <c r="BK126" t="n">
+        <v>98.7883640982027</v>
+      </c>
+      <c r="BL126" t="n">
+        <v>66.8624144413201</v>
+      </c>
+      <c r="BM126" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="BN126" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="BO126" t="n">
+        <v>47.2</v>
+      </c>
+      <c r="BP126" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="BQ126" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="BR126" t="n">
+        <v>55.2</v>
+      </c>
+      <c r="BS126" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="BT126" t="n">
+        <v>56.8</v>
+      </c>
+      <c r="BU126" t="n">
+        <v>78.4</v>
+      </c>
+      <c r="BV126" t="n">
+        <v>118</v>
+      </c>
+      <c r="BW126" t="n">
+        <v>56.6</v>
+      </c>
+      <c r="BX126" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="BY126" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="BZ126" t="n">
+        <v>74.5</v>
+      </c>
+      <c r="CA126" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="CB126" t="n">
+        <v>6</v>
+      </c>
+      <c r="CC126" t="n">
+        <v>9</v>
+      </c>
+      <c r="CD126" t="n">
+        <v>1.476</v>
+      </c>
+      <c r="CE126" t="n">
+        <v>0.603</v>
+      </c>
+      <c r="CF126" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="CG126" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="CH126" t="n">
+        <v>-13.9</v>
+      </c>
+      <c r="CI126" t="n">
+        <v>43.2</v>
+      </c>
+      <c r="CJ126" t="n">
+        <v>49</v>
+      </c>
+      <c r="CK126" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="CL126" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="CM126" t="n">
+        <v>46.8</v>
+      </c>
+      <c r="CN126" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="CO126" t="n">
+        <v>44.6</v>
+      </c>
+      <c r="CP126" t="n">
+        <v>66.2</v>
+      </c>
+      <c r="CQ126" t="n">
+        <v>99.4</v>
+      </c>
+      <c r="CR126" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="CS126" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="CT126" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="CU126" t="n">
+        <v>71.9</v>
+      </c>
+      <c r="CV126" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="CW126" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="CX126" t="n">
+        <v>0.927</v>
+      </c>
+      <c r="CY126" t="n">
+        <v>0.565</v>
+      </c>
+      <c r="CZ126" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="DA126" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="DB126" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="DC126" t="n">
+        <v>0.958</v>
+      </c>
+      <c r="DD126" t="n">
+        <v>0.923</v>
+      </c>
+      <c r="DE126" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="DF126" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="DG126" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>123</v>
+      </c>
+      <c r="B127" t="n">
+        <v>122.95885823211</v>
+      </c>
+      <c r="C127" t="n">
+        <v>94.6707539780454</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.735613786620976</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.603010895211314</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0.790845910588888</v>
+      </c>
+      <c r="G127" t="n">
+        <v>110.827153441749</v>
+      </c>
+      <c r="H127" t="n">
+        <v>99.1406160590647</v>
+      </c>
+      <c r="I127" t="n">
+        <v>71.8637683642112</v>
+      </c>
+      <c r="J127" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="K127" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="L127" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="M127" t="n">
+        <v>19.7</v>
+      </c>
+      <c r="N127" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="O127" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="P127" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="Q127" t="n">
+        <v>54.4</v>
+      </c>
+      <c r="R127" t="n">
+        <v>74.8</v>
+      </c>
+      <c r="S127" t="n">
+        <v>112.3</v>
+      </c>
+      <c r="T127" t="n">
+        <v>64</v>
+      </c>
+      <c r="U127" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="V127" t="n">
+        <v>40</v>
+      </c>
+      <c r="W127" t="n">
+        <v>73.1</v>
+      </c>
+      <c r="X127" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="Y127" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="Z127" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="AA127" t="n">
+        <v>1.652</v>
+      </c>
+      <c r="AB127" t="n">
+        <v>0.573</v>
+      </c>
+      <c r="AC127" t="n">
+        <v>12.7</v>
+      </c>
+      <c r="AD127" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE127" t="n">
+        <v>-13.2</v>
+      </c>
+      <c r="AF127" t="n">
+        <v>45.3</v>
+      </c>
+      <c r="AG127" t="n">
+        <v>48.8</v>
+      </c>
+      <c r="AH127" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI127" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="AJ127" t="n">
+        <v>47.7</v>
+      </c>
+      <c r="AK127" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="AL127" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="AM127" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="AN127" t="n">
+        <v>101.9</v>
+      </c>
+      <c r="AO127" t="n">
+        <v>59.9</v>
+      </c>
+      <c r="AP127" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="AQ127" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="AR127" t="n">
+        <v>60</v>
+      </c>
+      <c r="AS127" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="AT127" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AU127" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="AV127" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="AW127" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="AX127" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="AY127" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="AZ127" t="n">
+        <v>1.028</v>
+      </c>
+      <c r="BA127" t="n">
+        <v>0.952</v>
+      </c>
+      <c r="BB127" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="BC127" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="BD127" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE127" t="n">
+        <v>122.783517287024</v>
+      </c>
+      <c r="BF127" t="n">
+        <v>90.6258236924989</v>
+      </c>
+      <c r="BG127" t="n">
+        <v>0.7193970466841</v>
+      </c>
+      <c r="BH127" t="n">
+        <v>0.588201540444193</v>
+      </c>
+      <c r="BI127" t="n">
+        <v>0.756867952390836</v>
+      </c>
+      <c r="BJ127" t="n">
+        <v>109.739975952838</v>
+      </c>
+      <c r="BK127" t="n">
+        <v>98.6081868217284</v>
+      </c>
+      <c r="BL127" t="n">
+        <v>66.8585044477694</v>
+      </c>
+      <c r="BM127" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="BN127" t="n">
+        <v>52</v>
+      </c>
+      <c r="BO127" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="BP127" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="BQ127" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="BR127" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="BS127" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="BT127" t="n">
+        <v>57.3</v>
+      </c>
+      <c r="BU127" t="n">
+        <v>78.2</v>
+      </c>
+      <c r="BV127" t="n">
+        <v>119</v>
+      </c>
+      <c r="BW127" t="n">
+        <v>56.4</v>
+      </c>
+      <c r="BX127" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="BY127" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="BZ127" t="n">
+        <v>74.1</v>
+      </c>
+      <c r="CA127" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="CB127" t="n">
+        <v>6</v>
+      </c>
+      <c r="CC127" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="CD127" t="n">
+        <v>1.471</v>
+      </c>
+      <c r="CE127" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="CF127" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="CG127" t="n">
+        <v>22</v>
+      </c>
+      <c r="CH127" t="n">
+        <v>-14.7</v>
+      </c>
+      <c r="CI127" t="n">
+        <v>43.1</v>
+      </c>
+      <c r="CJ127" t="n">
+        <v>49</v>
+      </c>
+      <c r="CK127" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="CL127" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="CM127" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="CN127" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="CO127" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="CP127" t="n">
+        <v>66.1</v>
+      </c>
+      <c r="CQ127" t="n">
+        <v>98.8</v>
+      </c>
+      <c r="CR127" t="n">
+        <v>56</v>
+      </c>
+      <c r="CS127" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="CT127" t="n">
+        <v>25.9</v>
+      </c>
+      <c r="CU127" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="CV127" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="CW127" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="CX127" t="n">
+        <v>0.913</v>
+      </c>
+      <c r="CY127" t="n">
+        <v>0.562</v>
+      </c>
+      <c r="CZ127" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="DA127" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="DB127" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="DC127" t="n">
+        <v>0.957</v>
+      </c>
+      <c r="DD127" t="n">
+        <v>0.924</v>
+      </c>
+      <c r="DE127" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="DF127" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="DG127" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>